<commit_message>
Correcion de mensaje notificaion,otros
</commit_message>
<xml_diff>
--- a/app/src/main/resources/DOWNLOAD_PERSONAL_FICHAS.xlsx
+++ b/app/src/main/resources/DOWNLOAD_PERSONAL_FICHAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sigma\sigma_web_backend_api\app\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3FBB50-C44F-4F0C-ABD2-EC220071C8C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2350F2-C582-4CEC-9316-AC320B00B6E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5A150F25-885F-43DA-A656-DE7C92D3B68C}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>CODIGO</t>
-  </si>
-  <si>
     <t>NOMBRES</t>
   </si>
   <si>
@@ -63,10 +60,13 @@
     <t>OBSERVACIONES</t>
   </si>
   <si>
-    <t>REGISTRO FICHA</t>
-  </si>
-  <si>
     <t>FECHA</t>
+  </si>
+  <si>
+    <t>REGISTRO FICHA?</t>
+  </si>
+  <si>
+    <t>CODIGO FICHA</t>
   </si>
 </sst>
 </file>
@@ -517,13 +517,13 @@
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" style="1" customWidth="1"/>
     <col min="5" max="6" width="13.5703125" style="1" customWidth="1"/>
@@ -538,46 +538,46 @@
   <sheetData>
     <row r="1" spans="1:14" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>5</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>